<commit_message>
modified BOM for new version box
</commit_message>
<xml_diff>
--- a/BOMs/BOM.xlsx
+++ b/BOMs/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Item</t>
   </si>
@@ -123,22 +123,16 @@
     <t>Permatex 80050 Clear RTV Silicone Adhesive Sealant, 3 oz.</t>
   </si>
   <si>
-    <t>http://www.amazon.com/1000Pcs-M1-4x4-Plated-Electronic-Phillips/dp/B00HB1TTJ4/ref=sr_1_11?ie=UTF8&amp;qid=1405472514&amp;sr=8-11&amp;keywords=screw+m1.4</t>
-  </si>
-  <si>
-    <t>http://www.amazon.com/StarTech-Mounting-Computer-4-Inches-Standoff/dp/B00032Q1J4/ref=sr_1_1?ie=UTF8&amp;qid=1405472554&amp;sr=8-1&amp;keywords=screw+m3</t>
-  </si>
-  <si>
-    <t>M1.4x4 Screw </t>
-  </si>
-  <si>
-    <t>M3 Screw</t>
-  </si>
-  <si>
     <t>http://www.amazon.com/VELCRO-U-S-A-Sticky-Black-VEK91137/dp/B000GRBEK2/ref=sr_1_13?ie=UTF8&amp;qid=1405473316&amp;sr=8-13&amp;keywords=velcro+sticky+back+hook</t>
   </si>
   <si>
     <t>Velcro Sticky Back</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9609</t>
+  </si>
+  <si>
+    <t>Slide Switch</t>
   </si>
 </sst>
 </file>
@@ -529,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -598,7 +592,7 @@
         <v>6.95</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E13" si="0">B3 * D3</f>
+        <f t="shared" ref="E3:E12" si="0">B3 * D3</f>
         <v>6.95</v>
       </c>
       <c r="F3" s="3"/>
@@ -719,13 +713,13 @@
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3">
         <v>26.04</v>
@@ -738,126 +732,107 @@
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="D11" s="3">
-        <v>9.8699999999999992</v>
+        <v>0.75</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
-        <v>9.8699999999999992</v>
+        <v>0.75</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>36</v>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="3">
-        <v>3.99</v>
+        <v>1.95</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>3.99</v>
+        <v>1.95</v>
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1.95</v>
-      </c>
-      <c r="E13" s="3">
-        <f t="shared" si="0"/>
-        <v>1.95</v>
-      </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="2" t="s">
+    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="3">
-        <f>SUM(E2:E13)</f>
-        <v>139.44</v>
+      <c r="E14" s="3">
+        <f>SUM(E2:E12)</f>
+        <v>126.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>28</v>
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify BOM. change battery to 110mah
</commit_message>
<xml_diff>
--- a/BOMs/BOM.xlsx
+++ b/BOMs/BOM.xlsx
@@ -57,12 +57,6 @@
     <t>Arduino Pro Mini 328 - 3.3V/8MHz</t>
   </si>
   <si>
-    <t>https://www.sparkfun.com/products/10718</t>
-  </si>
-  <si>
-    <t>Polymer Lithium Ion Battery - 400mAh</t>
-  </si>
-  <si>
     <t>Triple Axis Accelerometer MMA7361</t>
   </si>
   <si>
@@ -133,6 +127,12 @@
   </si>
   <si>
     <t>Slide Switch</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/731</t>
+  </si>
+  <si>
+    <t>Polymer Lithium Ion Battery - 110mAh</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -580,20 +580,20 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3">
-        <v>6.95</v>
+        <v>4.95</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" ref="E3:E12" si="0">B3 * D3</f>
-        <v>6.95</v>
+        <v>4.95</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -637,13 +637,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
         <v>11.95</v>
@@ -656,13 +656,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3">
         <v>0.5</v>
@@ -675,13 +675,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3">
         <v>7.95</v>
@@ -694,13 +694,13 @@
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3">
         <v>4.3899999999999997</v>
@@ -713,13 +713,13 @@
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3">
         <v>26.04</v>
@@ -732,13 +732,13 @@
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3">
         <v>0.75</v>
@@ -751,13 +751,13 @@
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="3">
         <v>1.95</v>
@@ -778,62 +778,62 @@
       </c>
       <c r="E14" s="3">
         <f>SUM(E2:E12)</f>
-        <v>126.33</v>
+        <v>124.33</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>